<commit_message>
added NY, WA, LA, CA mitigation dates
</commit_message>
<xml_diff>
--- a/epidemiologypriors.xlsx
+++ b/epidemiologypriors.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aavattikutis/Git/covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74734A4B-C74B-514A-BDFC-7232F8F7191E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4EA8A5-D0DD-B444-AF7F-3FA34EA36753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
   </bookViews>
   <sheets>
     <sheet name="mitigation" sheetId="1" r:id="rId1"/>
+    <sheet name="mitigation sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>region</t>
   </si>
@@ -72,16 +73,42 @@
   </si>
   <si>
     <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>https://www.imperial.ac.uk/mrc-global-infectious-disease-analysis/covid-19/report-13-europe-npi-impact/</t>
+  </si>
+  <si>
+    <t>US_NY</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/mmwr/volumes/69/wr/mm6915e2.htm</t>
+  </si>
+  <si>
+    <t>US_LA</t>
+  </si>
+  <si>
+    <t>US_WA</t>
+  </si>
+  <si>
+    <t>US_CA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,14 +131,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6314A468-2D72-3E45-805A-E1B0EE0F6FF6}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +558,68 @@
         <v>43902</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF60C16-84DC-144F-8C7D-6E340746D0B6}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{008B47C5-2F8A-FA42-8315-A90614892101}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{9C565F78-F395-FF4E-ADB1-8C68FB670680}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mitigation dates for most states
</commit_message>
<xml_diff>
--- a/epidemiologypriors.xlsx
+++ b/epidemiologypriors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aavattikutis/Git/covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4EA8A5-D0DD-B444-AF7F-3FA34EA36753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14165825-7640-5540-997A-66BDF0DA56A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>region</t>
   </si>
@@ -91,6 +91,138 @@
   </si>
   <si>
     <t>US_CA</t>
+  </si>
+  <si>
+    <t>US_AL</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/interactive/2020/us/coronavirus-stay-at-home-order.html</t>
+  </si>
+  <si>
+    <t>US_AK</t>
+  </si>
+  <si>
+    <t>US_AZ</t>
+  </si>
+  <si>
+    <t>US_CO</t>
+  </si>
+  <si>
+    <t>US_CT</t>
+  </si>
+  <si>
+    <t>US_DE</t>
+  </si>
+  <si>
+    <t>US_DC</t>
+  </si>
+  <si>
+    <t>US_FL</t>
+  </si>
+  <si>
+    <t>US_GA</t>
+  </si>
+  <si>
+    <t>US_HI</t>
+  </si>
+  <si>
+    <t>US_ID</t>
+  </si>
+  <si>
+    <t>US_IL</t>
+  </si>
+  <si>
+    <t>US_IN</t>
+  </si>
+  <si>
+    <t>US_KY</t>
+  </si>
+  <si>
+    <t>US_KS</t>
+  </si>
+  <si>
+    <t>US_ME</t>
+  </si>
+  <si>
+    <t>US_MD</t>
+  </si>
+  <si>
+    <t>US_MA</t>
+  </si>
+  <si>
+    <t>US_MI</t>
+  </si>
+  <si>
+    <t>US_MN</t>
+  </si>
+  <si>
+    <t>US_MS</t>
+  </si>
+  <si>
+    <t>US_MO</t>
+  </si>
+  <si>
+    <t>US_MT</t>
+  </si>
+  <si>
+    <t>US_NV</t>
+  </si>
+  <si>
+    <t>US_NH</t>
+  </si>
+  <si>
+    <t>US_NJ</t>
+  </si>
+  <si>
+    <t>US_NM</t>
+  </si>
+  <si>
+    <t>US_NC</t>
+  </si>
+  <si>
+    <t>US_OH</t>
+  </si>
+  <si>
+    <t>US_OK</t>
+  </si>
+  <si>
+    <t>US_OR</t>
+  </si>
+  <si>
+    <t>US_PA</t>
+  </si>
+  <si>
+    <t>US_PR</t>
+  </si>
+  <si>
+    <t>US_RI</t>
+  </si>
+  <si>
+    <t>US_SC</t>
+  </si>
+  <si>
+    <t>US_TN</t>
+  </si>
+  <si>
+    <t>US_TX</t>
+  </si>
+  <si>
+    <t>US_UT</t>
+  </si>
+  <si>
+    <t>US_VT</t>
+  </si>
+  <si>
+    <t>US_VA</t>
+  </si>
+  <si>
+    <t>US_WV</t>
+  </si>
+  <si>
+    <t>US_WI</t>
+  </si>
+  <si>
+    <t>US_WY</t>
   </si>
 </sst>
 </file>
@@ -454,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6314A468-2D72-3E45-805A-E1B0EE0F6FF6}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,26 +692,26 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
-        <v>43902</v>
+        <v>43925</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
-        <v>43903</v>
+        <v>43918</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
-        <v>43905</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -587,7 +719,351 @@
         <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>43901</v>
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1">
+        <v>43916</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1">
+        <v>43916</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="1">
+        <v>43918</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="1">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1">
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="1">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="1">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="1">
+        <v>43918</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="1">
+        <v>43928</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="1">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="1">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="1">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="1">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="1">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="1">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="1">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="1">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="1">
+        <v>43918</v>
       </c>
     </row>
   </sheetData>
@@ -597,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF60C16-84DC-144F-8C7D-6E340746D0B6}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,10 +1091,16 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{008B47C5-2F8A-FA42-8315-A90614892101}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{9C565F78-F395-FF4E-ADB1-8C68FB670680}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{4D2BCCF3-7F9E-F248-8D73-72651D77A0B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added gamma mean and sd for death from two sources
</commit_message>
<xml_diff>
--- a/epidemiologypriors.xlsx
+++ b/epidemiologypriors.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aavattikutis/Git/covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14165825-7640-5540-997A-66BDF0DA56A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C92CE-71B9-3649-80A9-C69291F7405D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
   </bookViews>
   <sheets>
     <sheet name="mitigation" sheetId="1" r:id="rId1"/>
     <sheet name="mitigation sources" sheetId="2" r:id="rId2"/>
+    <sheet name="recovery_statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="death_statistics" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>region</t>
   </si>
@@ -81,9 +83,6 @@
     <t>US_NY</t>
   </si>
   <si>
-    <t>https://www.cdc.gov/mmwr/volumes/69/wr/mm6915e2.htm</t>
-  </si>
-  <si>
     <t>US_LA</t>
   </si>
   <si>
@@ -223,6 +222,21 @@
   </si>
   <si>
     <t>US_WY</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC7074197/</t>
+  </si>
+  <si>
+    <t>mean = 15, sd = 7</t>
+  </si>
+  <si>
+    <t>mean = 19, sd = 9</t>
   </si>
 </sst>
 </file>
@@ -267,10 +281,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6314A468-2D72-3E45-805A-E1B0EE0F6FF6}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
+    <sheetView topLeftCell="A50" zoomScale="249" zoomScaleNormal="249" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -692,7 +712,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>43925</v>
@@ -700,7 +720,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>43918</v>
@@ -708,7 +728,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>43921</v>
@@ -716,7 +736,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>43909</v>
@@ -724,7 +744,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>43916</v>
@@ -732,7 +752,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>43913</v>
@@ -740,7 +760,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <v>43914</v>
@@ -748,7 +768,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>43922</v>
@@ -756,7 +776,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
         <v>43924</v>
@@ -764,7 +784,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
         <v>43924</v>
@@ -772,7 +792,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1">
         <v>43915</v>
@@ -780,7 +800,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1">
         <v>43915</v>
@@ -788,7 +808,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1">
         <v>43911</v>
@@ -796,7 +816,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>43914</v>
@@ -804,7 +824,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1">
         <v>43920</v>
@@ -812,7 +832,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1">
         <v>43916</v>
@@ -820,7 +840,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1">
         <v>43913</v>
@@ -828,7 +848,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
         <v>43923</v>
@@ -836,7 +856,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="1">
         <v>43920</v>
@@ -844,7 +864,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1">
         <v>43914</v>
@@ -852,7 +872,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1">
         <v>43914</v>
@@ -860,7 +880,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1">
         <v>43917</v>
@@ -868,7 +888,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1">
         <v>43924</v>
@@ -876,7 +896,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1">
         <v>43927</v>
@@ -884,7 +904,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="1">
         <v>43918</v>
@@ -892,7 +912,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1">
         <v>43922</v>
@@ -900,7 +920,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1">
         <v>43917</v>
@@ -908,7 +928,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1">
         <v>43911</v>
@@ -916,7 +936,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="1">
         <v>43914</v>
@@ -932,7 +952,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1">
         <v>43920</v>
@@ -940,7 +960,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1">
         <v>43913</v>
@@ -948,7 +968,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1">
         <v>43915</v>
@@ -956,7 +976,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1">
         <v>43913</v>
@@ -964,7 +984,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1">
         <v>43922</v>
@@ -972,7 +992,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1">
         <v>43905</v>
@@ -980,7 +1000,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1">
         <v>43918</v>
@@ -988,7 +1008,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1">
         <v>43928</v>
@@ -996,7 +1016,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1">
         <v>43921</v>
@@ -1004,7 +1024,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" s="1">
         <v>43923</v>
@@ -1012,7 +1032,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" s="1">
         <v>43917</v>
@@ -1020,7 +1040,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" s="1">
         <v>43915</v>
@@ -1028,7 +1048,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="1">
         <v>43920</v>
@@ -1036,7 +1056,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B56" s="1">
         <v>43913</v>
@@ -1044,7 +1064,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" s="1">
         <v>43914</v>
@@ -1052,7 +1072,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" s="1">
         <v>43915</v>
@@ -1060,7 +1080,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" s="1">
         <v>43918</v>
@@ -1073,11 +1093,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF60C16-84DC-144F-8C7D-6E340746D0B6}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1088,19 +1106,72 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{008B47C5-2F8A-FA42-8315-A90614892101}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{9C565F78-F395-FF4E-ADB1-8C68FB670680}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{4D2BCCF3-7F9E-F248-8D73-72651D77A0B1}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{4D2BCCF3-7F9E-F248-8D73-72651D77A0B1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA69545-D5E7-FC44-9029-BCE0F650201F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="218" zoomScaleNormal="218" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A83E557-182E-3F42-99BA-C449A366DCB7}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{053E7264-AE77-B641-AC69-E73409D226DC}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{82472216-D163-4C43-A570-22C8CA69C706}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added ferguson priors for death and recovery, gamma mean and sd
</commit_message>
<xml_diff>
--- a/epidemiologypriors.xlsx
+++ b/epidemiologypriors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aavattikutis/Git/covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C92CE-71B9-3649-80A9-C69291F7405D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8E0DEB-9D43-A046-9396-11B79F5B15FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{82EA345B-DE0F-0F4A-A92C-513349F5FA3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>region</t>
   </si>
@@ -227,16 +227,28 @@
     <t>source</t>
   </si>
   <si>
-    <t>gamma</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC7074197/</t>
   </si>
   <si>
     <t>mean = 15, sd = 7</t>
   </si>
   <si>
-    <t>mean = 19, sd = 9</t>
+    <t>gamma death</t>
+  </si>
+  <si>
+    <t>gamma recovery</t>
+  </si>
+  <si>
+    <t>https://www.medrxiv.org/content/10.1101/2020.03.09.20033357v1.full.pdf</t>
+  </si>
+  <si>
+    <t>mean = 18.8, sd = 8.5</t>
+  </si>
+  <si>
+    <t>mean = 24.7, sd = 8.7</t>
+  </si>
+  <si>
+    <t>https://www.medrxiv.org/content/10.1101/2020.04.01.20050138v1.full.pdf</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A83E557-182E-3F42-99BA-C449A366DCB7}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,34 +1156,45 @@
     <col min="2" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{053E7264-AE77-B641-AC69-E73409D226DC}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{82472216-D163-4C43-A570-22C8CA69C706}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{6DE8C718-303F-5649-912B-23957BED7CEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>